<commit_message>
small updates on ExcelMergeIntoTemplate script
</commit_message>
<xml_diff>
--- a/data_import/template.xlsx
+++ b/data_import/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plindner/Development/NWC_backend/data_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA022E2F-DCC8-6A4C-8744-2C66F0AA490D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A2D3C9-A835-8444-9E98-FB8AB377F455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53940" yWindow="500" windowWidth="43620" windowHeight="21400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53940" yWindow="500" windowWidth="43620" windowHeight="21400" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Data" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,12 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Nancy Beck Young - Personal View" guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" mergeInterval="0" personalView="1" xWindow="1548" yWindow="-77" windowWidth="1673" windowHeight="850" activeSheetId="9"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" mergeInterval="0" personalView="1" maximized="1" yWindow="23" windowWidth="1366" windowHeight="679" activeSheetId="5"/>
+    <customWorkbookView name="Claude Willan - Personal View" guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1920" windowHeight="865" tabRatio="716" activeSheetId="4"/>
+    <customWorkbookView name="Zarnow, Leandra R - Personal View" guid="{C3874448-A812-8040-8431-8F21B0489AFC}" mergeInterval="0" personalView="1" windowWidth="1302" windowHeight="554" activeSheetId="1"/>
+    <customWorkbookView name="Dan Clason - Personal View" guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Nancy Young - Personal View" guid="{7132840B-F908-9041-87B8-CDBD763689F5}" mergeInterval="0" personalView="1" xWindow="1472" yWindow="-25" windowWidth="1865" windowHeight="990" activeSheetId="1"/>
-    <customWorkbookView name="Dan Clason - Personal View" guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Zarnow, Leandra R - Personal View" guid="{C3874448-A812-8040-8431-8F21B0489AFC}" mergeInterval="0" personalView="1" windowWidth="1302" windowHeight="554" activeSheetId="1"/>
-    <customWorkbookView name="Claude Willan - Personal View" guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1920" windowHeight="865" tabRatio="716" activeSheetId="4"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" mergeInterval="0" personalView="1" maximized="1" yWindow="23" windowWidth="1366" windowHeight="679" activeSheetId="5"/>
-    <customWorkbookView name="Nancy Beck Young - Personal View" guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" mergeInterval="0" personalView="1" xWindow="1548" yWindow="-77" windowWidth="1673" windowHeight="850" activeSheetId="9"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -220,9 +220,6 @@
     <t>Name of Political Offices Sought but Lost (if more than one, list all but create new row for each)</t>
   </si>
   <si>
-    <t xml:space="preserve">Year of Race that was Lost </t>
-  </si>
-  <si>
     <t>delegate, Democratic National Convention</t>
   </si>
   <si>
@@ -2552,6 +2549,9 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Year of Race that was Lost</t>
   </si>
 </sst>
 </file>
@@ -3184,7 +3184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3223,64 +3223,64 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>114</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N1" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>116</v>
-      </c>
-      <c r="P1" s="20" t="s">
-        <v>117</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="11" t="s">
         <v>745</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>746</v>
       </c>
       <c r="V1" s="11" t="s">
         <v>9</v>
@@ -3295,13 +3295,13 @@
         <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>5</v>
@@ -3312,19 +3312,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>13</v>
@@ -3336,7 +3336,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K2" s="19">
         <v>1933</v>
@@ -3345,7 +3345,7 @@
         <v>44</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N2" s="21">
         <v>12</v>
@@ -3378,7 +3378,7 @@
         <v>20</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>22</v>
@@ -3393,9 +3393,25 @@
     <sortCondition ref="A2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="150">
+    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="140">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:M1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="150">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4:E5"/>
+      <selection pane="bottomRight" activeCell="J44" sqref="J44"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+    </customSheetView>
+    <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="150">
+      <pane xSplit="2" ySplit="1.0079365079365079" topLeftCell="D36" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{C3874448-A812-8040-8431-8F21B0489AFC}" scale="150">
+      <selection activeCell="T3" sqref="T3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}">
@@ -3403,25 +3419,9 @@
       <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{C3874448-A812-8040-8431-8F21B0489AFC}" scale="150">
-      <selection activeCell="T3" sqref="T3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="150">
-      <pane xSplit="2" ySplit="1.0079365079365079" topLeftCell="D36" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="150">
+    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="150">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="J44" sqref="J44"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-    </customSheetView>
-    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="140">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:M1048576"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4:E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -3499,82 +3499,82 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
@@ -3584,85 +3584,85 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -3704,57 +3704,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>749</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>750</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>751</v>
-      </c>
       <c r="E1" s="26" t="s">
+        <v>763</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>816</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>760</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>764</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>817</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>761</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>765</v>
-      </c>
       <c r="I1" s="26" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>22</v>
@@ -3763,25 +3763,25 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="M2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3790,103 +3790,103 @@
         <v>26</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="L3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="M3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="26"/>
       <c r="B4" s="26" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="J4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="L4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="M4" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="26"/>
       <c r="B5" s="26" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D5" s="26"/>
       <c r="H5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I5" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="M5" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="H6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I6" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="L6" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="M6" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -3894,160 +3894,160 @@
         <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="L7" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="M7" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="M8" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I9" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="L9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="M9" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I10" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="L10" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="M10" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="L11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="L12" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="L13" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="L14" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="L15" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L16" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="L17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I18" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="19" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="20" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="21" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="22" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="23" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I23" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="24" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I24" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="25" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I25" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="26" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I26" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="27" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="28" spans="9:12" x14ac:dyDescent="0.2">
       <c r="I28" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
   </sheetData>
@@ -4073,31 +4073,31 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>741</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4105,7 +4105,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4139,22 +4139,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -4211,169 +4211,169 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="BB1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="BC1" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="BD1" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:57" ht="34" x14ac:dyDescent="0.2">
@@ -4617,19 +4617,19 @@
         <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -4643,7 +4643,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>27</v>
@@ -4667,7 +4667,7 @@
         <v>22</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>32</v>
@@ -4679,7 +4679,7 @@
         <v>45</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
@@ -4692,14 +4692,14 @@
     <sortCondition ref="B2:B3"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="160">
-      <pane xSplit="2" ySplit="1" topLeftCell="V36" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="133">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}" scale="130">
-      <pane xSplit="2" ySplit="0.50427350427350426" topLeftCell="C61" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
+    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="130">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="AM66" sqref="AM66"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="130">
@@ -4708,14 +4708,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="130">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="AM66" sqref="AM66"/>
+    <customSheetView guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}" scale="130">
+      <pane xSplit="2" ySplit="0.50427350427350426" topLeftCell="C61" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="133">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="160">
+      <pane xSplit="2" ySplit="1" topLeftCell="V36" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4748,11 +4748,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1:O1048576"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4779,10 +4779,10 @@
         <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>49</v>
@@ -4791,7 +4791,7 @@
         <v>50</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>51</v>
+        <v>828</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>7</v>
@@ -4800,7 +4800,7 @@
         <v>14</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>18</v>
@@ -4821,10 +4821,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3">
         <v>1980</v>
@@ -4833,13 +4833,13 @@
         <v>1980</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="J2" s="3">
         <v>1992</v>
@@ -4870,9 +4870,19 @@
     <sortCondition ref="K2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="130">
-      <pane xSplit="2" ySplit="1" topLeftCell="H33" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="120">
+      <pane xSplit="2" ySplit="1" topLeftCell="C60" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="160">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="160">
+      <pane xSplit="2" ySplit="1.0046296296296295" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}" scale="160">
@@ -4880,19 +4890,9 @@
       <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="160">
-      <pane xSplit="2" ySplit="1.0046296296296295" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="160">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="120">
-      <pane xSplit="2" ySplit="1" topLeftCell="C60" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="130">
+      <pane xSplit="2" ySplit="1" topLeftCell="H33" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4946,13 +4946,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="102" x14ac:dyDescent="0.2">
@@ -4963,13 +4963,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -5008,1567 +5008,1567 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CD1" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="CG1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="CH1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="CI1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="CJ1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="CK1" s="3" t="s">
+      <c r="CL1" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CM1" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="CM1" s="3" t="s">
+      <c r="CN1" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="CN1" s="3" t="s">
+      <c r="CO1" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="CQ1" s="3" t="s">
+      <c r="CR1" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="CU1" s="3" t="s">
+      <c r="CV1" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="CV1" s="3" t="s">
+      <c r="CW1" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="CW1" s="3" t="s">
+      <c r="CX1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="CX1" s="3" t="s">
+      <c r="CY1" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="CY1" s="8" t="s">
+      <c r="CZ1" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="CZ1" s="3" t="s">
+      <c r="DA1" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="DA1" s="3" t="s">
+      <c r="DB1" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="DB1" s="3" t="s">
+      <c r="DC1" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="DC1" s="3" t="s">
+      <c r="DD1" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="DD1" s="3" t="s">
+      <c r="DE1" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="DE1" s="3" t="s">
+      <c r="DF1" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="DF1" s="3" t="s">
+      <c r="DG1" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="DG1" s="3" t="s">
+      <c r="DH1" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="DH1" s="3" t="s">
+      <c r="DI1" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="DI1" s="3" t="s">
+      <c r="DJ1" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="DJ1" s="3" t="s">
+      <c r="DK1" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="DK1" s="3" t="s">
+      <c r="DL1" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="DL1" s="3" t="s">
+      <c r="DM1" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DN1" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="DN1" s="3" t="s">
+      <c r="DO1" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="DO1" s="3" t="s">
+      <c r="DP1" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DQ1" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="DQ1" s="3" t="s">
+      <c r="DR1" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="DR1" s="3" t="s">
+      <c r="DS1" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="DS1" s="3" t="s">
+      <c r="DT1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="DT1" s="3" t="s">
+      <c r="DU1" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="DU1" s="3" t="s">
+      <c r="DV1" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="DV1" s="3" t="s">
+      <c r="DW1" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="DW1" s="3" t="s">
+      <c r="DX1" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="DX1" s="3" t="s">
+      <c r="DY1" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="DZ1" s="2" t="s">
+      <c r="EA1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="EA1" s="3" t="s">
+      <c r="EB1" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="EB1" s="3" t="s">
+      <c r="EC1" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="EC1" s="3" t="s">
+      <c r="ED1" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="ED1" s="3" t="s">
+      <c r="EE1" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="EE1" s="3" t="s">
+      <c r="EF1" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="EF1" s="3" t="s">
+      <c r="EG1" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="EG1" s="3" t="s">
+      <c r="EH1" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="EH1" s="3" t="s">
+      <c r="EI1" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="EI1" s="3" t="s">
+      <c r="EJ1" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="EJ1" s="3" t="s">
+      <c r="EK1" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="EK1" s="3" t="s">
+      <c r="EL1" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="EL1" s="3" t="s">
+      <c r="EM1" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="EM1" s="3" t="s">
+      <c r="EN1" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="EN1" s="3" t="s">
+      <c r="EO1" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="EO1" s="3" t="s">
+      <c r="EP1" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="EP1" s="3" t="s">
+      <c r="EQ1" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="EQ1" s="3" t="s">
+      <c r="ER1" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="ER1" s="3" t="s">
+      <c r="ES1" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="ES1" s="2" t="s">
+      <c r="ET1" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="ET1" s="3" t="s">
+      <c r="EU1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="EU1" s="3" t="s">
+      <c r="EV1" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="EV1" s="3" t="s">
+      <c r="EW1" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="EW1" s="3" t="s">
+      <c r="EX1" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="EX1" s="3" t="s">
+      <c r="EY1" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="EY1" s="3" t="s">
+      <c r="EZ1" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="EZ1" s="3" t="s">
+      <c r="FA1" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="FA1" s="3" t="s">
+      <c r="FB1" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="FB1" s="3" t="s">
+      <c r="FC1" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="FC1" s="3" t="s">
+      <c r="FD1" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="FD1" s="2" t="s">
+      <c r="FE1" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="FE1" s="3" t="s">
+      <c r="FF1" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="FF1" s="3" t="s">
+      <c r="FG1" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="FG1" s="3" t="s">
+      <c r="FH1" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="FH1" s="3" t="s">
+      <c r="FI1" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="FI1" s="3" t="s">
+      <c r="FJ1" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="FJ1" s="3" t="s">
+      <c r="FK1" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="FK1" s="3" t="s">
+      <c r="FL1" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="FL1" s="3" t="s">
+      <c r="FM1" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="FM1" s="3" t="s">
+      <c r="FN1" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="FN1" s="3" t="s">
+      <c r="FO1" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="FO1" s="3" t="s">
+      <c r="FP1" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="FP1" s="2" t="s">
+      <c r="FQ1" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="FQ1" s="3" t="s">
+      <c r="FR1" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="FR1" s="3" t="s">
+      <c r="FS1" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="FS1" s="3" t="s">
+      <c r="FT1" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="FT1" s="3" t="s">
+      <c r="FU1" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="FU1" s="3" t="s">
+      <c r="FV1" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="FV1" s="3" t="s">
+      <c r="FW1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="FW1" s="3" t="s">
+      <c r="FX1" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="FX1" s="3" t="s">
+      <c r="FY1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="FY1" s="3" t="s">
+      <c r="FZ1" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="FZ1" s="2" t="s">
+      <c r="GA1" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="GA1" s="3" t="s">
+      <c r="GB1" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="GB1" s="3" t="s">
+      <c r="GC1" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="GC1" s="3" t="s">
+      <c r="GD1" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="GD1" s="3" t="s">
+      <c r="GE1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="GE1" s="3" t="s">
+      <c r="GF1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="GF1" s="3" t="s">
+      <c r="GG1" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="GG1" s="3" t="s">
+      <c r="GH1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="GH1" s="3" t="s">
+      <c r="GI1" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="GI1" s="3" t="s">
+      <c r="GJ1" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="GJ1" s="3" t="s">
+      <c r="GK1" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="GK1" s="3" t="s">
+      <c r="GL1" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="GL1" s="3" t="s">
+      <c r="GM1" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="GM1" s="3" t="s">
+      <c r="GN1" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="GN1" s="3" t="s">
+      <c r="GO1" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="GO1" s="3" t="s">
+      <c r="GP1" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="GP1" s="3" t="s">
+      <c r="GQ1" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="GQ1" s="3" t="s">
+      <c r="GR1" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="GR1" s="3" t="s">
+      <c r="GS1" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="GS1" s="3" t="s">
+      <c r="GT1" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="GT1" s="2" t="s">
+      <c r="GU1" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="GU1" s="3" t="s">
+      <c r="GV1" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="GV1" s="3" t="s">
+      <c r="GW1" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="GW1" s="3" t="s">
+      <c r="GX1" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="GX1" s="3" t="s">
+      <c r="GY1" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="GY1" s="3" t="s">
+      <c r="GZ1" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="GZ1" s="3" t="s">
+      <c r="HA1" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="HA1" s="3" t="s">
+      <c r="HB1" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="HB1" s="3" t="s">
+      <c r="HC1" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="HC1" s="3" t="s">
+      <c r="HD1" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="HD1" s="3" t="s">
+      <c r="HE1" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="HE1" s="2" t="s">
+      <c r="HF1" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="HF1" s="3" t="s">
+      <c r="HG1" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="HG1" s="3" t="s">
+      <c r="HH1" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="HH1" s="3" t="s">
+      <c r="HI1" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="HI1" s="3" t="s">
+      <c r="HJ1" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="HJ1" s="2" t="s">
+      <c r="HK1" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="HK1" s="3" t="s">
+      <c r="HL1" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="HL1" s="2" t="s">
+      <c r="HM1" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="HM1" s="3" t="s">
+      <c r="HN1" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="HN1" s="3" t="s">
+      <c r="HO1" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="HO1" s="3" t="s">
+      <c r="HP1" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="HP1" s="3" t="s">
+      <c r="HQ1" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="HQ1" s="3" t="s">
+      <c r="HR1" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="HR1" s="3" t="s">
+      <c r="HS1" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="HS1" s="3" t="s">
+      <c r="HT1" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="HT1" s="3" t="s">
+      <c r="HU1" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="HU1" s="3" t="s">
+      <c r="HV1" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="HV1" s="3" t="s">
+      <c r="HW1" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="HW1" s="3" t="s">
+      <c r="HX1" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="HX1" s="3" t="s">
+      <c r="HY1" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="HY1" s="3" t="s">
+      <c r="HZ1" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="HZ1" s="3" t="s">
+      <c r="IA1" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="IA1" s="3" t="s">
+      <c r="IB1" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="IB1" s="3" t="s">
+      <c r="IC1" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="IC1" s="3" t="s">
+      <c r="ID1" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="ID1" s="3" t="s">
+      <c r="IE1" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="IE1" s="3" t="s">
+      <c r="IF1" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="IF1" s="3" t="s">
+      <c r="IG1" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="IG1" s="3" t="s">
+      <c r="IH1" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="IH1" s="3" t="s">
+      <c r="II1" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="II1" s="3" t="s">
+      <c r="IJ1" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="IJ1" s="3" t="s">
+      <c r="IK1" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="IK1" s="3" t="s">
+      <c r="IL1" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="IL1" s="3" t="s">
+      <c r="IM1" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="IM1" s="3" t="s">
+      <c r="IN1" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="IN1" s="3" t="s">
+      <c r="IO1" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="IO1" s="3" t="s">
+      <c r="IP1" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="IP1" s="3" t="s">
+      <c r="IQ1" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="IQ1" s="3" t="s">
+      <c r="IR1" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="IR1" s="3" t="s">
+      <c r="IS1" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="IS1" s="3" t="s">
+      <c r="IT1" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="IT1" s="3" t="s">
+      <c r="IU1" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="IU1" s="3" t="s">
+      <c r="IV1" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="IV1" s="3" t="s">
+      <c r="IW1" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="IW1" s="3" t="s">
+      <c r="IX1" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="IX1" s="3" t="s">
+      <c r="IY1" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="IY1" s="3" t="s">
+      <c r="IZ1" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="IZ1" s="3" t="s">
+      <c r="JA1" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="JA1" s="3" t="s">
+      <c r="JB1" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="JB1" s="3" t="s">
+      <c r="JC1" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="JC1" s="3" t="s">
+      <c r="JD1" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="JD1" s="3" t="s">
+      <c r="JE1" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="JE1" s="3" t="s">
+      <c r="JF1" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="JF1" s="3" t="s">
+      <c r="JG1" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="JG1" s="3" t="s">
+      <c r="JH1" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="JH1" s="3" t="s">
+      <c r="JI1" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="JI1" s="3" t="s">
+      <c r="JJ1" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="JJ1" s="2" t="s">
+      <c r="JK1" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="JK1" s="3" t="s">
+      <c r="JL1" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="JL1" s="3" t="s">
+      <c r="JM1" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="JM1" s="3" t="s">
+      <c r="JN1" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="JN1" s="3" t="s">
+      <c r="JO1" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="JO1" s="3" t="s">
+      <c r="JP1" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="JP1" s="3" t="s">
+      <c r="JQ1" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="JQ1" s="3" t="s">
+      <c r="JR1" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="JR1" s="3" t="s">
+      <c r="JS1" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="JS1" s="3" t="s">
+      <c r="JT1" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="JT1" s="3" t="s">
+      <c r="JU1" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="JU1" s="2" t="s">
+      <c r="JV1" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="JV1" s="3" t="s">
+      <c r="JW1" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="JW1" s="3" t="s">
+      <c r="JX1" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="JX1" s="3" t="s">
+      <c r="JY1" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="JY1" s="3" t="s">
+      <c r="JZ1" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="JZ1" s="3" t="s">
+      <c r="KA1" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="KA1" s="3" t="s">
+      <c r="KB1" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="KB1" s="3" t="s">
+      <c r="KC1" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="KC1" s="3" t="s">
+      <c r="KD1" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="KD1" s="3" t="s">
+      <c r="KE1" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="KE1" s="3" t="s">
+      <c r="KF1" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="KF1" s="3" t="s">
+      <c r="KG1" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="KG1" s="3" t="s">
+      <c r="KH1" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="KH1" s="3" t="s">
+      <c r="KI1" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="KI1" s="3" t="s">
+      <c r="KJ1" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="KJ1" s="3" t="s">
+      <c r="KK1" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="KK1" s="3" t="s">
+      <c r="KL1" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="KL1" s="2" t="s">
+      <c r="KM1" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="KM1" s="3" t="s">
+      <c r="KN1" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="KN1" s="3" t="s">
+      <c r="KO1" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="KO1" s="2" t="s">
+      <c r="KP1" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="KP1" s="3" t="s">
+      <c r="KQ1" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="KQ1" s="3" t="s">
+      <c r="KR1" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="KR1" s="2" t="s">
+      <c r="KS1" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="KS1" s="3" t="s">
+      <c r="KT1" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="KT1" s="3" t="s">
+      <c r="KU1" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="KU1" s="3" t="s">
+      <c r="KV1" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="KV1" s="2" t="s">
+      <c r="KW1" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="KW1" s="2" t="s">
+      <c r="KX1" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="KX1" s="2" t="s">
+      <c r="KY1" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="KY1" s="3" t="s">
+      <c r="KZ1" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="KZ1" s="3" t="s">
+      <c r="LA1" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="LA1" s="3" t="s">
+      <c r="LB1" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="LB1" s="3" t="s">
+      <c r="LC1" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="LC1" s="2" t="s">
+      <c r="LD1" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="LD1" s="3" t="s">
+      <c r="LE1" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="LE1" s="3" t="s">
+      <c r="LF1" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="LF1" s="3" t="s">
+      <c r="LG1" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="LG1" s="3" t="s">
+      <c r="LH1" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="LH1" s="3" t="s">
+      <c r="LI1" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="LI1" s="3" t="s">
+      <c r="LJ1" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="LJ1" s="3" t="s">
+      <c r="LK1" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="LK1" s="3" t="s">
+      <c r="LL1" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="LL1" s="3" t="s">
+      <c r="LM1" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="LM1" s="3" t="s">
+      <c r="LN1" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="LN1" s="3" t="s">
+      <c r="LO1" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="LO1" s="3" t="s">
+      <c r="LP1" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="LP1" s="3" t="s">
+      <c r="LQ1" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="LQ1" s="3" t="s">
+      <c r="LR1" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="LR1" s="3" t="s">
+      <c r="LS1" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="LS1" s="3" t="s">
+      <c r="LT1" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="LT1" s="3" t="s">
+      <c r="LU1" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="LU1" s="3" t="s">
+      <c r="LV1" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="LV1" s="3" t="s">
+      <c r="LW1" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="LW1" s="3" t="s">
+      <c r="LX1" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="LX1" s="3" t="s">
+      <c r="LY1" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="LY1" s="3" t="s">
+      <c r="LZ1" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="LZ1" s="3" t="s">
+      <c r="MA1" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="MA1" s="3" t="s">
+      <c r="MB1" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="MB1" s="3" t="s">
+      <c r="MC1" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="MC1" s="3" t="s">
+      <c r="MD1" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="MD1" s="3" t="s">
+      <c r="ME1" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="ME1" s="3" t="s">
+      <c r="MF1" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="MF1" s="3" t="s">
+      <c r="MG1" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="MG1" s="3" t="s">
+      <c r="MH1" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="MH1" s="3" t="s">
+      <c r="MI1" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="MI1" s="3" t="s">
+      <c r="MJ1" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="MJ1" s="3" t="s">
+      <c r="MK1" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="MK1" s="3" t="s">
+      <c r="ML1" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="ML1" s="3" t="s">
+      <c r="MM1" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="MM1" s="2" t="s">
+      <c r="MN1" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="MN1" s="3" t="s">
+      <c r="MO1" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="MO1" s="3" t="s">
+      <c r="MP1" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="MP1" s="3" t="s">
+      <c r="MQ1" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="MQ1" s="3" t="s">
+      <c r="MR1" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="MR1" s="3" t="s">
+      <c r="MS1" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="MS1" s="3" t="s">
+      <c r="MT1" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="MT1" s="4" t="s">
+      <c r="MU1" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="MU1" s="3" t="s">
+      <c r="MV1" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="MV1" s="3" t="s">
+      <c r="MW1" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="MW1" s="3" t="s">
+      <c r="MX1" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="MX1" s="3" t="s">
+      <c r="MY1" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="MY1" s="3" t="s">
+      <c r="MZ1" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="MZ1" s="3" t="s">
+      <c r="NA1" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="NA1" s="3" t="s">
+      <c r="NB1" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="NB1" s="3" t="s">
+      <c r="NC1" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="NC1" s="3" t="s">
+      <c r="ND1" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="ND1" s="3" t="s">
+      <c r="NE1" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="NE1" s="3" t="s">
+      <c r="NF1" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="NF1" s="3" t="s">
+      <c r="NG1" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="NG1" s="2" t="s">
+      <c r="NH1" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="NH1" s="3" t="s">
+      <c r="NI1" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="NI1" s="3" t="s">
+      <c r="NJ1" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="NJ1" s="3" t="s">
+      <c r="NK1" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="NK1" s="3" t="s">
+      <c r="NL1" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="NL1" s="3" t="s">
+      <c r="NM1" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="NM1" s="3" t="s">
+      <c r="NN1" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="NN1" s="3" t="s">
+      <c r="NO1" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="NO1" s="3" t="s">
+      <c r="NP1" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="NP1" s="3" t="s">
+      <c r="NQ1" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="NQ1" s="3" t="s">
+      <c r="NR1" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="NR1" s="3" t="s">
+      <c r="NS1" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="NS1" s="3" t="s">
+      <c r="NT1" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="NT1" s="3" t="s">
+      <c r="NU1" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="NU1" s="3" t="s">
+      <c r="NV1" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="NV1" s="3" t="s">
+      <c r="NW1" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="NW1" s="3" t="s">
+      <c r="NX1" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="NX1" s="3" t="s">
+      <c r="NY1" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="NY1" s="3" t="s">
+      <c r="NZ1" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="NZ1" s="3" t="s">
+      <c r="OA1" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="OA1" s="3" t="s">
+      <c r="OB1" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="OB1" s="3" t="s">
+      <c r="OC1" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="OC1" s="3" t="s">
+      <c r="OD1" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="OD1" s="3" t="s">
+      <c r="OE1" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="OE1" s="3" t="s">
+      <c r="OF1" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="OF1" s="3" t="s">
+      <c r="OG1" s="3" t="s">
         <v>607</v>
       </c>
-      <c r="OG1" s="3" t="s">
+      <c r="OH1" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="OH1" s="3" t="s">
+      <c r="OI1" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="OI1" s="3" t="s">
+      <c r="OJ1" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="OJ1" s="3" t="s">
+      <c r="OK1" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="OK1" s="3" t="s">
+      <c r="OL1" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="OL1" s="3" t="s">
+      <c r="OM1" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="OM1" s="3" t="s">
+      <c r="ON1" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="ON1" s="3" t="s">
+      <c r="OO1" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="OO1" s="3" t="s">
+      <c r="OP1" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="OP1" s="3" t="s">
+      <c r="OQ1" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="OQ1" s="3" t="s">
+      <c r="OR1" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="OR1" s="3" t="s">
+      <c r="OS1" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="OS1" s="3" t="s">
+      <c r="OT1" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="OT1" s="3" t="s">
+      <c r="OU1" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="OU1" s="3" t="s">
+      <c r="OV1" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="OV1" s="3" t="s">
+      <c r="OW1" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="OW1" s="3" t="s">
+      <c r="OX1" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="OX1" s="3" t="s">
+      <c r="OY1" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="OY1" s="3" t="s">
+      <c r="OZ1" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="OZ1" s="3" t="s">
+      <c r="PA1" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="PA1" s="3" t="s">
+      <c r="PB1" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="PB1" s="3" t="s">
+      <c r="PC1" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="PC1" s="3" t="s">
+      <c r="PD1" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="PD1" s="3" t="s">
+      <c r="PE1" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="PE1" s="3" t="s">
+      <c r="PF1" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="PF1" s="3" t="s">
+      <c r="PG1" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="PG1" s="3" t="s">
+      <c r="PH1" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="PH1" s="3" t="s">
+      <c r="PI1" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="PI1" s="3" t="s">
+      <c r="PJ1" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="PJ1" s="3" t="s">
+      <c r="PK1" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="PK1" s="3" t="s">
+      <c r="PL1" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="PL1" s="3" t="s">
+      <c r="PM1" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="PM1" s="3" t="s">
+      <c r="PN1" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="PN1" s="3" t="s">
+      <c r="PO1" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="PO1" s="3" t="s">
+      <c r="PP1" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="PP1" s="3" t="s">
+      <c r="PQ1" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="PQ1" s="2" t="s">
+      <c r="PR1" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="PR1" s="3" t="s">
+      <c r="PS1" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="PS1" s="3" t="s">
+      <c r="PT1" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="PT1" s="3" t="s">
+      <c r="PU1" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="PU1" s="3" t="s">
+      <c r="PV1" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="PV1" s="3" t="s">
+      <c r="PW1" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="PW1" s="3" t="s">
+      <c r="PX1" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="PX1" s="3" t="s">
+      <c r="PY1" s="3" t="s">
         <v>651</v>
       </c>
-      <c r="PY1" s="3" t="s">
+      <c r="PZ1" s="3" t="s">
         <v>652</v>
       </c>
-      <c r="PZ1" s="3" t="s">
+      <c r="QA1" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="QA1" s="3" t="s">
+      <c r="QB1" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="QB1" s="3" t="s">
+      <c r="QC1" s="3" t="s">
         <v>655</v>
       </c>
-      <c r="QC1" s="3" t="s">
+      <c r="QD1" s="3" t="s">
         <v>656</v>
       </c>
-      <c r="QD1" s="3" t="s">
+      <c r="QE1" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="QE1" s="3" t="s">
+      <c r="QF1" s="3" t="s">
         <v>658</v>
       </c>
-      <c r="QF1" s="3" t="s">
+      <c r="QG1" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="QG1" s="3" t="s">
+      <c r="QH1" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="QH1" s="3" t="s">
+      <c r="QI1" s="3" t="s">
         <v>661</v>
       </c>
-      <c r="QI1" s="3" t="s">
+      <c r="QJ1" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="QJ1" s="3" t="s">
+      <c r="QK1" s="3" t="s">
         <v>663</v>
       </c>
-      <c r="QK1" s="3" t="s">
+      <c r="QL1" s="3" t="s">
         <v>664</v>
       </c>
-      <c r="QL1" s="3" t="s">
+      <c r="QM1" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="QM1" s="3" t="s">
+      <c r="QN1" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="QN1" s="3" t="s">
+      <c r="QO1" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="QO1" s="3" t="s">
+      <c r="QP1" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="QP1" s="3" t="s">
+      <c r="QQ1" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="QQ1" s="3" t="s">
+      <c r="QR1" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="QR1" s="3" t="s">
+      <c r="QS1" s="3" t="s">
         <v>671</v>
       </c>
-      <c r="QS1" s="3" t="s">
+      <c r="QT1" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="QT1" s="3" t="s">
+      <c r="QU1" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="QU1" s="3" t="s">
+      <c r="QV1" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="QV1" s="3" t="s">
+      <c r="QW1" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="QW1" s="3" t="s">
+      <c r="QX1" s="3" t="s">
         <v>676</v>
       </c>
-      <c r="QX1" s="3" t="s">
+      <c r="QY1" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="QY1" s="3" t="s">
+      <c r="QZ1" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="QZ1" s="3" t="s">
+      <c r="RA1" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="RA1" s="3" t="s">
+      <c r="RB1" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="RB1" s="3" t="s">
+      <c r="RC1" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="RC1" s="3" t="s">
+      <c r="RD1" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="RD1" s="3" t="s">
+      <c r="RE1" s="3" t="s">
         <v>683</v>
       </c>
-      <c r="RE1" s="3" t="s">
+      <c r="RF1" s="3" t="s">
         <v>684</v>
       </c>
-      <c r="RF1" s="3" t="s">
+      <c r="RG1" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="RG1" s="3" t="s">
+      <c r="RH1" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="RH1" s="3" t="s">
+      <c r="RI1" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="RI1" s="3" t="s">
+      <c r="RJ1" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="RJ1" s="3" t="s">
+      <c r="RK1" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="RK1" s="3" t="s">
+      <c r="RL1" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="RL1" s="3" t="s">
+      <c r="RM1" s="3" t="s">
         <v>691</v>
       </c>
-      <c r="RM1" s="3" t="s">
+      <c r="RN1" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="RN1" s="3" t="s">
+      <c r="RO1" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="RO1" s="3" t="s">
+      <c r="RP1" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="RP1" s="3" t="s">
+      <c r="RQ1" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="RQ1" s="3" t="s">
+      <c r="RR1" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="RR1" s="3" t="s">
+      <c r="RS1" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="RS1" s="3" t="s">
+      <c r="RT1" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="RT1" s="2" t="s">
+      <c r="RU1" s="3" t="s">
         <v>699</v>
       </c>
-      <c r="RU1" s="3" t="s">
+      <c r="RV1" s="3" t="s">
         <v>700</v>
       </c>
-      <c r="RV1" s="3" t="s">
+      <c r="RW1" s="3" t="s">
         <v>701</v>
       </c>
-      <c r="RW1" s="3" t="s">
+      <c r="RX1" s="3" t="s">
         <v>702</v>
       </c>
-      <c r="RX1" s="3" t="s">
+      <c r="RY1" s="3" t="s">
         <v>703</v>
       </c>
-      <c r="RY1" s="3" t="s">
+      <c r="RZ1" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="RZ1" s="3" t="s">
+      <c r="SA1" s="3" t="s">
         <v>705</v>
       </c>
-      <c r="SA1" s="3" t="s">
+      <c r="SB1" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="SB1" s="3" t="s">
+      <c r="SC1" s="3" t="s">
         <v>707</v>
       </c>
-      <c r="SC1" s="3" t="s">
+      <c r="SD1" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="SD1" s="3" t="s">
+      <c r="SE1" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="SE1" s="3" t="s">
+      <c r="SF1" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="SF1" s="3" t="s">
+      <c r="SG1" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="SG1" s="3" t="s">
+      <c r="SH1" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="SH1" s="3" t="s">
+      <c r="SI1" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="SI1" s="3" t="s">
+      <c r="SJ1" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="SJ1" s="3" t="s">
+      <c r="SK1" s="3" t="s">
         <v>715</v>
       </c>
-      <c r="SK1" s="3" t="s">
+      <c r="SL1" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="SL1" s="3" t="s">
+      <c r="SM1" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="SM1" s="3" t="s">
+      <c r="SN1" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="SN1" s="3" t="s">
+      <c r="SO1" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="SO1" s="3" t="s">
+      <c r="SP1" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="SP1" s="3" t="s">
+      <c r="SQ1" s="3" t="s">
         <v>721</v>
       </c>
-      <c r="SQ1" s="3" t="s">
+      <c r="SR1" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="SR1" s="3" t="s">
+      <c r="SS1" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="SS1" s="3" t="s">
+      <c r="ST1" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="ST1" s="2" t="s">
+      <c r="SU1" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="SU1" s="4" t="s">
+      <c r="SV1" s="4" t="s">
         <v>726</v>
       </c>
-      <c r="SV1" s="4" t="s">
+      <c r="SW1" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="SW1" s="4" t="s">
+      <c r="SX1" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="SX1" s="4" t="s">
+      <c r="SY1" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="SY1" s="4" t="s">
+      <c r="SZ1" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="SZ1" s="4" t="s">
+      <c r="TA1" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="TA1" s="4" t="s">
+      <c r="TB1" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="TB1" s="4" t="s">
+      <c r="TC1" s="4" t="s">
         <v>733</v>
-      </c>
-      <c r="TC1" s="4" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="2" spans="1:523" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -6576,7 +6576,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>22</v>
@@ -8210,115 +8210,115 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y1" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z1" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA1" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB1" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD1" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE1" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="AH1" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI1" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK1" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:41" ht="34" x14ac:dyDescent="0.2">
@@ -8497,9 +8497,19 @@
     <sortCondition ref="B2:B74"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="150">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="150">
+      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="H55" sqref="H55"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="150">
+      <pane xSplit="2" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="150">
+      <pane xSplit="2" ySplit="1.0055555555555555" topLeftCell="C57" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="G51" sqref="G51"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{0C71D9B9-0C4F-4C06-B246-E9F55F8F57C4}" scale="150">
@@ -8507,19 +8517,9 @@
       <selection pane="bottomRight" activeCell="C1" sqref="C1:E1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{177EE23F-EF35-7247-B68F-A5848D6162F2}" scale="150">
-      <pane xSplit="2" ySplit="1.0055555555555555" topLeftCell="C57" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="G51" sqref="G51"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{D7AC6949-A4B3-814F-B95B-281DFB2434BD}" scale="150">
-      <pane xSplit="2" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A581424C-CB35-5E44-8508-DDCCFB1C8F33}" scale="150">
-      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="H55" sqref="H55"/>
+    <customSheetView guid="{7132840B-F908-9041-87B8-CDBD763689F5}" scale="150">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -8779,6 +8779,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="bd76514a-38d3-4a55-a838-849dda26f7e2" xsi:nil="true"/>
@@ -8787,15 +8796,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8818,6 +8818,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A39BC44-814E-415D-89CF-22C6CCD92E2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3745846C-53CD-4FBE-AA4C-FA2DA17DDEF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="bd76514a-38d3-4a55-a838-849dda26f7e2"/>
@@ -8832,12 +8840,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A39BC44-814E-415D-89CF-22C6CCD92E2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>